<commit_message>
Incorporate wind cost curves by state provided by Yuyu.
</commit_message>
<xml_diff>
--- a/rgcam-data-system/rgcam-data/Assumptions/Tables_Res_Data.xlsx
+++ b/rgcam-data-system/rgcam-data/Assumptions/Tables_Res_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8680" yWindow="3380" windowWidth="25360" windowHeight="15820" tabRatio="500" firstSheet="6" activeTab="10"/>
+    <workbookView xWindow="8680" yWindow="3380" windowWidth="25360" windowHeight="15820" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <externalReference r:id="rId13"/>
     <externalReference r:id="rId14"/>
     <externalReference r:id="rId15"/>
+    <externalReference r:id="rId16"/>
   </externalReferences>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="88">
   <si>
     <t>This workbook collects resource assumptions from various sources</t>
   </si>
@@ -290,6 +291,15 @@
   </si>
   <si>
     <t>electricity_sector_market</t>
+  </si>
+  <si>
+    <t>large onshore windresource</t>
+  </si>
+  <si>
+    <t>large onshore wind</t>
+  </si>
+  <si>
+    <t>subResourceVariance</t>
   </si>
 </sst>
 </file>
@@ -369,11 +379,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="232">
+  <cellStyleXfs count="244">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -613,7 +635,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="232">
+  <cellStyles count="244">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -729,6 +751,12 @@
     <cellStyle name="Followed Hyperlink" xfId="227" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="229" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="231" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="233" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="235" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="237" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="239" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="241" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="243" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -844,6 +872,12 @@
     <cellStyle name="Hyperlink" xfId="226" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="228" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="230" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="232" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="234" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="236" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="238" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="240" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="242" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3"/>
   </cellStyles>
@@ -1295,6 +1329,41 @@
       <sheetData sheetId="5"/>
       <sheetData sheetId="6"/>
       <sheetData sheetId="7"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink5.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Notes"/>
+      <sheetName val="TechCost"/>
+      <sheetName val="MaxResource"/>
+      <sheetName val="Transmission_cost"/>
+      <sheetName val="global_wind_input_ref"/>
+      <sheetName val="global_wind_adv"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4">
+        <row r="219">
+          <cell r="D219">
+            <v>0</v>
+          </cell>
+          <cell r="F219">
+            <v>0.3</v>
+          </cell>
+          <cell r="G219">
+            <v>0.4</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1622,10 +1691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1668,126 +1737,146 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1" t="s">
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
         <v>29</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="1" t="s">
+      <c r="A11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>45</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C13" t="s">
         <v>2</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D13" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
         <v>34</v>
       </c>
-      <c r="B15" t="s">
-        <v>34</v>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
         <v>34</v>
       </c>
-      <c r="B16" t="s">
-        <v>36</v>
+      <c r="B17" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" t="s">
-        <v>72</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
         <v>34</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
         <v>36</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C22" t="s">
         <v>36</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D22" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1850,15 +1939,15 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="str">
-        <f>Legend!A19</f>
+        <f>Legend!A21</f>
         <v>elect_td_bld</v>
       </c>
       <c r="B4" t="str">
-        <f>Legend!B19</f>
+        <f>Legend!B21</f>
         <v>elect_td_bld</v>
       </c>
       <c r="C4" t="str">
-        <f>Legend!C19</f>
+        <f>Legend!C21</f>
         <v>elect_td_bld</v>
       </c>
       <c r="D4">
@@ -1876,7 +1965,7 @@
         <v>3.03</v>
       </c>
       <c r="H4" t="str">
-        <f>Legend!D19</f>
+        <f>Legend!D21</f>
         <v>electricity_net_ownuse</v>
       </c>
       <c r="I4" t="s">
@@ -2173,15 +2262,15 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="str">
-        <f>Legend!A20</f>
+        <f>Legend!A22</f>
         <v>elect_td_bld</v>
       </c>
       <c r="B13" t="str">
-        <f>Legend!B20</f>
+        <f>Legend!B22</f>
         <v>rooftop_pv</v>
       </c>
       <c r="C13" t="str">
-        <f>Legend!C20</f>
+        <f>Legend!C22</f>
         <v>rooftop_pv</v>
       </c>
       <c r="D13">
@@ -2197,7 +2286,7 @@
         <v>0</v>
       </c>
       <c r="H13" t="str">
-        <f>Legend!D20</f>
+        <f>Legend!D22</f>
         <v>distributed_solar</v>
       </c>
       <c r="I13" t="s">
@@ -2498,7 +2587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
@@ -2557,15 +2646,15 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" t="str">
-        <f>Legend!A20</f>
+        <f>Legend!A22</f>
         <v>elect_td_bld</v>
       </c>
       <c r="B4" t="str">
-        <f>Legend!B20</f>
+        <f>Legend!B22</f>
         <v>rooftop_pv</v>
       </c>
       <c r="C4" t="str">
-        <f>Legend!C20</f>
+        <f>Legend!C22</f>
         <v>rooftop_pv</v>
       </c>
       <c r="D4">
@@ -3015,7 +3104,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3086,11 +3174,11 @@
         <v>27</v>
       </c>
       <c r="B6" t="str">
-        <f>Legend!A12</f>
+        <f>Legend!A14</f>
         <v>elect_td_bld</v>
       </c>
       <c r="C6" t="str">
-        <f>Legend!A11</f>
+        <f>Legend!A13</f>
         <v>sector</v>
       </c>
     </row>
@@ -3106,7 +3194,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
@@ -3174,8 +3262,26 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="str">
+        <f>Legend!A6</f>
+        <v>large onshore windresource</v>
+      </c>
+      <c r="B6" t="str">
+        <f>Legend!B6</f>
+        <v>EJ</v>
+      </c>
+      <c r="C6" t="str">
+        <f>Legend!C6</f>
+        <v>1975$/GJ</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3232,11 +3338,11 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="str">
-        <f>Legend!A8</f>
+        <f>Legend!A9</f>
         <v>geothermal</v>
       </c>
       <c r="B4" t="str">
-        <f>Legend!B8</f>
+        <f>Legend!B9</f>
         <v>hydrothermal</v>
       </c>
       <c r="C4">
@@ -3266,11 +3372,11 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="str">
-        <f>Legend!A9</f>
+        <f>Legend!A10</f>
         <v>distributed_solar</v>
       </c>
       <c r="B5" t="str">
-        <f>Legend!B9</f>
+        <f>Legend!B10</f>
         <v>distributed_solar</v>
       </c>
       <c r="C5">
@@ -3313,7 +3419,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3347,11 +3453,11 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="str">
-        <f>Legend!A8</f>
+        <f>Legend!A9</f>
         <v>geothermal</v>
       </c>
       <c r="B4" t="str">
-        <f>Legend!B8</f>
+        <f>Legend!B9</f>
         <v>hydrothermal</v>
       </c>
       <c r="C4" t="s">
@@ -3398,25 +3504,25 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -3429,14 +3535,17 @@
       <c r="D3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="str">
-        <f>Legend!A9</f>
+        <f>Legend!A10</f>
         <v>distributed_solar</v>
       </c>
       <c r="B4" t="str">
-        <f>Legend!B9</f>
+        <f>Legend!B10</f>
         <v>distributed_solar</v>
       </c>
       <c r="C4">
@@ -3447,9 +3556,35 @@
         <f>[2]rooftop_resource_input!$G$37</f>
         <v>0.2</v>
       </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="str">
+        <f>Legend!A11</f>
+        <v>large onshore windresource</v>
+      </c>
+      <c r="B5" t="str">
+        <f>Legend!B11</f>
+        <v>large onshore wind</v>
+      </c>
+      <c r="C5">
+        <f>[5]global_wind_input_ref!$D$219</f>
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <f>[5]global_wind_input_ref!$G$219</f>
+        <v>0.4</v>
+      </c>
+      <c r="E5">
+        <f>[5]global_wind_input_ref!$F$219</f>
+        <v>0.3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3504,19 +3639,19 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="str">
-        <f>Legend!A12</f>
+        <f>Legend!A14</f>
         <v>elect_td_bld</v>
       </c>
       <c r="B4" t="str">
-        <f>Legend!B12</f>
+        <f>Legend!B14</f>
         <v>EJ</v>
       </c>
       <c r="C4" t="str">
-        <f>Legend!C12</f>
+        <f>Legend!C14</f>
         <v>EJ</v>
       </c>
       <c r="D4" t="str">
-        <f>Legend!D12</f>
+        <f>Legend!D14</f>
         <v>1975$/GJ</v>
       </c>
       <c r="E4">
@@ -3593,11 +3728,11 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="str">
-        <f>Legend!A15</f>
+        <f>Legend!A17</f>
         <v>elect_td_bld</v>
       </c>
       <c r="B4" t="str">
-        <f>Legend!B15</f>
+        <f>Legend!B17</f>
         <v>elect_td_bld</v>
       </c>
       <c r="C4" s="6">
@@ -3624,11 +3759,11 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="str">
-        <f>Legend!A16</f>
+        <f>Legend!A18</f>
         <v>elect_td_bld</v>
       </c>
       <c r="B5" t="str">
-        <f>Legend!B16</f>
+        <f>Legend!B18</f>
         <v>rooftop_pv</v>
       </c>
       <c r="C5" s="6">
@@ -3711,11 +3846,11 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="str">
-        <f>Legend!A15</f>
+        <f>Legend!A17</f>
         <v>elect_td_bld</v>
       </c>
       <c r="B4" t="str">
-        <f>Legend!B15</f>
+        <f>Legend!B17</f>
         <v>elect_td_bld</v>
       </c>
       <c r="C4" s="6">
@@ -3739,11 +3874,11 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="str">
-        <f>Legend!A16</f>
+        <f>Legend!A18</f>
         <v>elect_td_bld</v>
       </c>
       <c r="B5" t="str">
-        <f>Legend!B16</f>
+        <f>Legend!B18</f>
         <v>rooftop_pv</v>
       </c>
       <c r="C5" s="6">

</xml_diff>